<commit_message>
update: alterada tela de sobre nos
</commit_message>
<xml_diff>
--- a/docs/documentacao/BackLogPI.xlsx
+++ b/docs/documentacao/BackLogPI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/949a7e447c1476a4/Documentos/AIRCONOMICS/AirConomics/docs/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{114AB4B1-ACF8-4C0D-AC1C-2F4527E071A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{114AB4B1-ACF8-4C0D-AC1C-2F4527E071A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EBC4F9-CB95-40D6-BEB4-DB795902A5E5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -819,7 +819,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,6 +876,12 @@
       <color rgb="FF000000"/>
       <name val="Aptos"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1176,7 +1182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1298,19 +1304,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1337,9 +1331,6 @@
     <xf numFmtId="164" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1358,15 +1349,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2822,64 +2827,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="65" style="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
       <c r="K1" s="38"/>
       <c r="L1" s="39"/>
       <c r="M1" s="39"/>
-      <c r="N1" s="56" t="s">
+      <c r="N1" s="65" t="s">
         <v>240</v>
       </c>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -2919,22 +2924,22 @@
       <c r="M2" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-    </row>
-    <row r="3" spans="1:27" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="58"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+    </row>
+    <row r="3" spans="1:27" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
         <v>11</v>
       </c>
@@ -2974,26 +2979,26 @@
       <c r="M3" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="N3" s="59" t="s">
+      <c r="N3" s="54" t="s">
         <v>241</v>
       </c>
-      <c r="O3" s="59" t="s">
+      <c r="O3" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
-      <c r="AA3" s="43"/>
-    </row>
-    <row r="4" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+    </row>
+    <row r="4" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>11</v>
       </c>
@@ -3033,26 +3038,26 @@
       <c r="M4" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="N4" s="55" t="s">
         <v>243</v>
       </c>
-      <c r="O4" s="60" t="s">
+      <c r="O4" s="55" t="s">
         <v>244</v>
       </c>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-    </row>
-    <row r="5" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+    </row>
+    <row r="5" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>11</v>
       </c>
@@ -3092,26 +3097,26 @@
       <c r="M5" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="N5" s="61" t="s">
+      <c r="N5" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="O5" s="61" t="s">
+      <c r="O5" s="56" t="s">
         <v>246</v>
       </c>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
-      <c r="AA5" s="43"/>
-    </row>
-    <row r="6" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="41"/>
+    </row>
+    <row r="6" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>11</v>
       </c>
@@ -3151,26 +3156,26 @@
       <c r="M6" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="N6" s="60" t="s">
+      <c r="N6" s="55" t="s">
         <v>247</v>
       </c>
-      <c r="O6" s="60" t="s">
+      <c r="O6" s="55" t="s">
         <v>248</v>
       </c>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="43"/>
-      <c r="Z6" s="43"/>
-      <c r="AA6" s="43"/>
-    </row>
-    <row r="7" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+    </row>
+    <row r="7" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>11</v>
       </c>
@@ -3210,26 +3215,26 @@
       <c r="M7" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="N7" s="61" t="s">
+      <c r="N7" s="56" t="s">
         <v>249</v>
       </c>
-      <c r="O7" s="61" t="s">
+      <c r="O7" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="43"/>
-      <c r="AA7" s="43"/>
-    </row>
-    <row r="8" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+    </row>
+    <row r="8" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
@@ -3269,26 +3274,26 @@
       <c r="M8" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="N8" s="60" t="s">
+      <c r="N8" s="55" t="s">
         <v>251</v>
       </c>
-      <c r="O8" s="60" t="s">
+      <c r="O8" s="55" t="s">
         <v>252</v>
       </c>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="43"/>
-      <c r="Y8" s="43"/>
-      <c r="Z8" s="43"/>
-      <c r="AA8" s="43"/>
-    </row>
-    <row r="9" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="57"/>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="41"/>
+    </row>
+    <row r="9" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>29</v>
       </c>
@@ -3328,22 +3333,22 @@
       <c r="M9" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-    </row>
-    <row r="10" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="41"/>
+    </row>
+    <row r="10" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>29</v>
       </c>
@@ -3383,22 +3388,22 @@
       <c r="M10" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="43"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="43"/>
-      <c r="AA10" s="43"/>
-    </row>
-    <row r="11" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="60"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="41"/>
+    </row>
+    <row r="11" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -3438,22 +3443,22 @@
       <c r="M11" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="64"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-    </row>
-    <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="60"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="41"/>
+    </row>
+    <row r="12" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -3493,22 +3498,22 @@
       <c r="M12" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43"/>
-    </row>
-    <row r="13" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="Z12" s="41"/>
+      <c r="AA12" s="41"/>
+    </row>
+    <row r="13" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -3548,22 +3553,22 @@
       <c r="M13" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="43"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="43"/>
-    </row>
-    <row r="14" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="41"/>
+    </row>
+    <row r="14" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -3603,22 +3608,22 @@
       <c r="M14" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64"/>
-      <c r="S14" s="64"/>
-      <c r="T14" s="43"/>
-      <c r="U14" s="43"/>
-      <c r="V14" s="43"/>
-      <c r="W14" s="43"/>
-      <c r="X14" s="43"/>
-      <c r="Y14" s="43"/>
-      <c r="Z14" s="43"/>
-      <c r="AA14" s="43"/>
-    </row>
-    <row r="15" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="41"/>
+    </row>
+    <row r="15" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -3658,22 +3663,22 @@
       <c r="M15" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="43"/>
-      <c r="T15" s="43"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="43"/>
-      <c r="X15" s="43"/>
-      <c r="Y15" s="43"/>
-      <c r="Z15" s="43"/>
-      <c r="AA15" s="43"/>
-    </row>
-    <row r="16" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="41"/>
+      <c r="W15" s="41"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="41"/>
+    </row>
+    <row r="16" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -3713,22 +3718,22 @@
       <c r="M16" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="43"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="43"/>
-      <c r="X16" s="43"/>
-      <c r="Y16" s="43"/>
-      <c r="Z16" s="43"/>
-      <c r="AA16" s="43"/>
-    </row>
-    <row r="17" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="Z16" s="41"/>
+      <c r="AA16" s="41"/>
+    </row>
+    <row r="17" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
@@ -3768,26 +3773,26 @@
       <c r="M17" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="57" t="s">
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="44" t="s">
+      <c r="Q17" s="53"/>
+      <c r="R17" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="S17" s="45"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="43"/>
-      <c r="X17" s="43"/>
-      <c r="Y17" s="43"/>
-      <c r="Z17" s="43"/>
-      <c r="AA17" s="43"/>
-    </row>
-    <row r="18" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="S17" s="64"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
+      <c r="Z17" s="41"/>
+      <c r="AA17" s="41"/>
+    </row>
+    <row r="18" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -3827,31 +3832,31 @@
       <c r="M18" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="46" t="s">
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="Q18" s="46">
+      <c r="Q18" s="42">
         <f>SUM(Q19:Q21)</f>
         <v>532</v>
       </c>
-      <c r="R18" s="47" t="s">
+      <c r="R18" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="S18" s="47">
+      <c r="S18" s="43">
         <v>370</v>
       </c>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="43"/>
-    </row>
-    <row r="19" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="41"/>
+    </row>
+    <row r="19" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -3879,8 +3884,8 @@
       <c r="I19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="24" t="s">
-        <v>63</v>
+      <c r="J19" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="K19" s="37" t="s">
         <v>197</v>
@@ -3891,31 +3896,31 @@
       <c r="M19" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="48" t="s">
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="Q19" s="48">
+      <c r="Q19" s="44">
         <f>SUM(G34:G69)</f>
         <v>196</v>
       </c>
-      <c r="R19" s="49" t="s">
+      <c r="R19" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="S19" s="49">
+      <c r="S19" s="45">
         <v>150</v>
       </c>
-      <c r="T19" s="43"/>
-      <c r="U19" s="43"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="43"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="43"/>
-      <c r="AA19" s="43"/>
-    </row>
-    <row r="20" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41"/>
+      <c r="Z19" s="41"/>
+      <c r="AA19" s="41"/>
+    </row>
+    <row r="20" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
@@ -3955,31 +3960,31 @@
       <c r="M20" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="50" t="s">
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="Q20" s="51">
+      <c r="Q20" s="47">
         <f>SUM(G18:G33)</f>
         <v>178</v>
       </c>
-      <c r="R20" s="49" t="s">
+      <c r="R20" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="S20" s="49">
+      <c r="S20" s="45">
         <v>100</v>
       </c>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="43"/>
-      <c r="X20" s="43"/>
-      <c r="Y20" s="43"/>
-      <c r="Z20" s="43"/>
-      <c r="AA20" s="43"/>
-    </row>
-    <row r="21" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41"/>
+      <c r="Z20" s="41"/>
+      <c r="AA20" s="41"/>
+    </row>
+    <row r="21" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
@@ -4019,31 +4024,31 @@
       <c r="M21" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="52" t="s">
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" s="53">
+      <c r="Q21" s="49">
         <f>SUM(G3:G17)</f>
         <v>158</v>
       </c>
-      <c r="R21" s="49" t="s">
+      <c r="R21" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="S21" s="49">
+      <c r="S21" s="45">
         <v>50</v>
       </c>
-      <c r="T21" s="43"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="43"/>
-      <c r="W21" s="43"/>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="43"/>
-      <c r="Z21" s="43"/>
-      <c r="AA21" s="43"/>
-    </row>
-    <row r="22" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41"/>
+      <c r="Z21" s="41"/>
+      <c r="AA21" s="41"/>
+    </row>
+    <row r="22" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -4083,27 +4088,27 @@
       <c r="M22" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="54" t="s">
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="Q22" s="55">
+      <c r="Q22" s="51">
         <f>AVERAGE(Q19:Q21)</f>
         <v>177.33333333333334</v>
       </c>
-      <c r="R22" s="43"/>
-      <c r="S22" s="43"/>
-      <c r="T22" s="43"/>
-      <c r="U22" s="43"/>
-      <c r="V22" s="43"/>
-      <c r="W22" s="43"/>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="43"/>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="43"/>
-    </row>
-    <row r="23" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="41"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="41"/>
+    </row>
+    <row r="23" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -4143,22 +4148,22 @@
       <c r="M23" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="43"/>
-      <c r="U23" s="43"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="43"/>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="43"/>
-    </row>
-    <row r="24" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="41"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41"/>
+      <c r="Z23" s="41"/>
+      <c r="AA23" s="41"/>
+    </row>
+    <row r="24" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>71</v>
       </c>
@@ -4198,22 +4203,22 @@
       <c r="M24" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="43"/>
-      <c r="T24" s="43"/>
-      <c r="U24" s="43"/>
-      <c r="V24" s="43"/>
-      <c r="W24" s="43"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="43"/>
-    </row>
-    <row r="25" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="41"/>
+      <c r="V24" s="41"/>
+      <c r="W24" s="41"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="41"/>
+      <c r="Z24" s="41"/>
+      <c r="AA24" s="41"/>
+    </row>
+    <row r="25" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
@@ -4253,22 +4258,22 @@
       <c r="M25" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="43"/>
-      <c r="T25" s="43"/>
-      <c r="U25" s="43"/>
-      <c r="V25" s="43"/>
-      <c r="W25" s="43"/>
-      <c r="X25" s="43"/>
-      <c r="Y25" s="43"/>
-      <c r="Z25" s="43"/>
-      <c r="AA25" s="43"/>
-    </row>
-    <row r="26" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="41"/>
+      <c r="W25" s="41"/>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41"/>
+      <c r="Z25" s="41"/>
+      <c r="AA25" s="41"/>
+    </row>
+    <row r="26" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>71</v>
       </c>
@@ -4308,22 +4313,22 @@
       <c r="M26" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="43"/>
-      <c r="T26" s="43"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="43"/>
-      <c r="W26" s="43"/>
-      <c r="X26" s="43"/>
-      <c r="Y26" s="43"/>
-      <c r="Z26" s="43"/>
-      <c r="AA26" s="43"/>
-    </row>
-    <row r="27" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+      <c r="T26" s="41"/>
+      <c r="U26" s="41"/>
+      <c r="V26" s="41"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41"/>
+      <c r="Z26" s="41"/>
+      <c r="AA26" s="41"/>
+    </row>
+    <row r="27" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -4363,22 +4368,22 @@
       <c r="M27" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="43"/>
-      <c r="Z27" s="43"/>
-      <c r="AA27" s="43"/>
-    </row>
-    <row r="28" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="41"/>
+    </row>
+    <row r="28" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -4418,22 +4423,22 @@
       <c r="M28" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="43"/>
-      <c r="U28" s="43"/>
-      <c r="V28" s="43"/>
-      <c r="W28" s="43"/>
-      <c r="X28" s="43"/>
-      <c r="Y28" s="43"/>
-      <c r="Z28" s="43"/>
-      <c r="AA28" s="43"/>
-    </row>
-    <row r="29" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="41"/>
+      <c r="V28" s="41"/>
+      <c r="W28" s="41"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="41"/>
+      <c r="Z28" s="41"/>
+      <c r="AA28" s="41"/>
+    </row>
+    <row r="29" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -4473,22 +4478,22 @@
       <c r="M29" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="43"/>
-      <c r="U29" s="43"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="43"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="43"/>
-      <c r="Z29" s="43"/>
-      <c r="AA29" s="43"/>
-    </row>
-    <row r="30" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="41"/>
+      <c r="AA29" s="41"/>
+    </row>
+    <row r="30" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
@@ -4516,8 +4521,8 @@
       <c r="I30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J30" s="22" t="s">
-        <v>18</v>
+      <c r="J30" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="K30" s="37" t="s">
         <v>208</v>
@@ -4528,22 +4533,22 @@
       <c r="M30" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="43"/>
-      <c r="Z30" s="43"/>
-      <c r="AA30" s="43"/>
-    </row>
-    <row r="31" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="41"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41"/>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="41"/>
+    </row>
+    <row r="31" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>40</v>
       </c>
@@ -4571,8 +4576,8 @@
       <c r="I31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J31" s="22" t="s">
-        <v>18</v>
+      <c r="J31" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="K31" s="37" t="s">
         <v>209</v>
@@ -4583,22 +4588,22 @@
       <c r="M31" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-      <c r="U31" s="43"/>
-      <c r="V31" s="43"/>
-      <c r="W31" s="43"/>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="43"/>
-      <c r="Z31" s="43"/>
-      <c r="AA31" s="43"/>
-    </row>
-    <row r="32" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
+      <c r="V31" s="41"/>
+      <c r="W31" s="41"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+      <c r="Z31" s="41"/>
+      <c r="AA31" s="41"/>
+    </row>
+    <row r="32" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>50</v>
       </c>
@@ -4626,8 +4631,8 @@
       <c r="I32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="22" t="s">
-        <v>18</v>
+      <c r="J32" s="66" t="s">
+        <v>59</v>
       </c>
       <c r="K32" s="37" t="s">
         <v>210</v>
@@ -4638,22 +4643,22 @@
       <c r="M32" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="43"/>
-      <c r="U32" s="43"/>
-      <c r="V32" s="43"/>
-      <c r="W32" s="43"/>
-      <c r="X32" s="43"/>
-      <c r="Y32" s="43"/>
-      <c r="Z32" s="43"/>
-      <c r="AA32" s="43"/>
-    </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="41"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="41"/>
+      <c r="Z32" s="41"/>
+      <c r="AA32" s="41"/>
+    </row>
+    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
@@ -4694,7 +4699,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>92</v>
       </c>
@@ -4735,7 +4740,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>92</v>
       </c>
@@ -4776,7 +4781,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>97</v>
       </c>
@@ -4817,7 +4822,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>97</v>
       </c>
@@ -4858,7 +4863,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>97</v>
       </c>
@@ -4899,7 +4904,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>97</v>
       </c>
@@ -4940,7 +4945,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>97</v>
       </c>
@@ -4981,7 +4986,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>97</v>
       </c>
@@ -5022,7 +5027,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>97</v>
       </c>
@@ -5063,7 +5068,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>92</v>
       </c>
@@ -5104,7 +5109,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>113</v>
       </c>
@@ -5145,7 +5150,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>71</v>
       </c>
@@ -5186,7 +5191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>71</v>
       </c>
@@ -5227,7 +5232,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>120</v>
       </c>
@@ -5268,7 +5273,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>71</v>
       </c>
@@ -5309,7 +5314,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>71</v>
       </c>
@@ -5350,7 +5355,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>71</v>
       </c>
@@ -5391,7 +5396,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>71</v>
       </c>
@@ -5432,7 +5437,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>71</v>
       </c>
@@ -5473,7 +5478,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>71</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>71</v>
       </c>
@@ -5555,7 +5560,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>71</v>
       </c>
@@ -5596,7 +5601,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>71</v>
       </c>
@@ -5637,7 +5642,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>71</v>
       </c>
@@ -5678,7 +5683,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>71</v>
       </c>
@@ -5719,7 +5724,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>36</v>
       </c>
@@ -5760,7 +5765,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>36</v>
       </c>
@@ -5801,7 +5806,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>36</v>
       </c>
@@ -5842,7 +5847,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>36</v>
       </c>
@@ -5883,7 +5888,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>36</v>
       </c>
@@ -5924,7 +5929,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
@@ -5965,7 +5970,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>155</v>
       </c>
@@ -6006,7 +6011,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>158</v>
       </c>
@@ -6047,7 +6052,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>158</v>
       </c>
@@ -6088,7 +6093,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>155</v>
       </c>
@@ -6129,7 +6134,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>155</v>
       </c>
@@ -6170,7 +6175,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I70" s="18"/>
       <c r="J70" s="18"/>
     </row>

</xml_diff>

<commit_message>
att diagrama e site
</commit_message>
<xml_diff>
--- a/docs/documentacao/BackLogPI.xlsx
+++ b/docs/documentacao/BackLogPI.xlsx
@@ -1,42 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/949a7e447c1476a4/Documentos/AIRCONOMICS/AirConomics/docs/documentacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avell\OneDrive\Área de Trabalho\facudade SPTECH\AirConomics\AirConomics\docs\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{114AB4B1-ACF8-4C0D-AC1C-2F4527E071A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EBC4F9-CB95-40D6-BEB4-DB795902A5E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6530A7BA-D1E0-4B4D-85DF-CE8C447EDE3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$2:$AA$69</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="252">
   <si>
     <t>AIRCONOMICS - BACKLOG</t>
   </si>
@@ -230,9 +222,6 @@
   </si>
   <si>
     <t>Planilha de Riscos do Projeto</t>
-  </si>
-  <si>
-    <t>ANDAMENTO</t>
   </si>
   <si>
     <t>SP1</t>
@@ -819,7 +808,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,13 +867,15 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -918,12 +909,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1182,7 +1167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1247,25 +1232,19 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1295,10 +1274,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1337,13 +1316,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1354,10 +1333,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1366,10 +1345,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2825,66 +2804,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="68.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65" style="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.8984375" customWidth="1"/>
+    <col min="2" max="2" width="20.59765625" customWidth="1"/>
+    <col min="3" max="3" width="68.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.8984375" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" customWidth="1"/>
+    <col min="10" max="10" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="65" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.8984375" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.3984375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="44.3984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:27" ht="26.25" customHeight="1">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="65" t="s">
-        <v>240</v>
-      </c>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -2916,37 +2896,37 @@
         <v>10</v>
       </c>
       <c r="K2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="L2" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="M2" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-    </row>
-    <row r="3" spans="1:27" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+      <c r="N2" s="56"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+    </row>
+    <row r="3" spans="1:27" ht="29.25" hidden="1" customHeight="1" thickBot="1">
+      <c r="A3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="12" t="s">
@@ -2955,57 +2935,57 @@
       <c r="E3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="33">
         <v>3</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="33">
         <v>1</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="37" t="s">
-        <v>170</v>
+      <c r="K3" s="35" t="s">
+        <v>169</v>
       </c>
       <c r="L3" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M3" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M3" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="N3" s="54" t="s">
+      <c r="N3" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="O3" s="52" t="s">
         <v>241</v>
       </c>
-      <c r="O3" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="41"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="41"/>
-    </row>
-    <row r="4" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+    </row>
+    <row r="4" spans="1:27" ht="29.25" hidden="1" customHeight="1">
+      <c r="A4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="12" t="s">
@@ -3014,57 +2994,57 @@
       <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="33">
         <v>3</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="33">
         <v>1</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M4" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="N4" s="55" t="s">
+      <c r="N4" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="O4" s="53" t="s">
         <v>243</v>
       </c>
-      <c r="O4" s="55" t="s">
-        <v>244</v>
-      </c>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="41"/>
-    </row>
-    <row r="5" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="39"/>
+    </row>
+    <row r="5" spans="1:27" ht="29.25" hidden="1" customHeight="1">
+      <c r="A5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="30" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -3073,57 +3053,57 @@
       <c r="E5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="33">
         <v>5</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="33">
         <v>2</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M5" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="L5" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="54" t="s">
+        <v>244</v>
+      </c>
+      <c r="O5" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="O5" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="41"/>
-    </row>
-    <row r="6" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="P5" s="55"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
+      <c r="AA5" s="39"/>
+    </row>
+    <row r="6" spans="1:27" ht="29.25" hidden="1" customHeight="1">
+      <c r="A6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -3132,57 +3112,57 @@
       <c r="E6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="33">
         <v>3</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="33">
         <v>3</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M6" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="L6" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="N6" s="55" t="s">
+      <c r="N6" s="53" t="s">
+        <v>246</v>
+      </c>
+      <c r="O6" s="53" t="s">
         <v>247</v>
       </c>
-      <c r="O6" s="55" t="s">
-        <v>248</v>
-      </c>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-    </row>
-    <row r="7" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
+    </row>
+    <row r="7" spans="1:27" ht="29.25" hidden="1" customHeight="1">
+      <c r="A7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -3191,57 +3171,57 @@
       <c r="E7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="33">
         <v>5</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="33">
         <v>1</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M7" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="L7" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="N7" s="56" t="s">
+      <c r="N7" s="54" t="s">
+        <v>248</v>
+      </c>
+      <c r="O7" s="54" t="s">
         <v>249</v>
       </c>
-      <c r="O7" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-    </row>
-    <row r="8" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="55"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="39"/>
+      <c r="Z7" s="39"/>
+      <c r="AA7" s="39"/>
+    </row>
+    <row r="8" spans="1:27" ht="29.25" hidden="1" customHeight="1">
+      <c r="A8" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -3250,57 +3230,57 @@
       <c r="E8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="33">
         <v>3</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="33">
         <v>2</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M8" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="L8" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="N8" s="55" t="s">
+      <c r="N8" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="O8" s="53" t="s">
         <v>251</v>
       </c>
-      <c r="O8" s="55" t="s">
-        <v>252</v>
-      </c>
-      <c r="P8" s="57"/>
-      <c r="Q8" s="57"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-    </row>
-    <row r="9" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="39"/>
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="39"/>
+    </row>
+    <row r="9" spans="1:27" ht="29.25" hidden="1" customHeight="1">
+      <c r="A9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="32" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -3309,53 +3289,53 @@
       <c r="E9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="33">
         <v>13</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="33">
         <v>1</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M9" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="L9" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="41"/>
-    </row>
-    <row r="10" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="39"/>
+      <c r="Z9" s="39"/>
+      <c r="AA9" s="39"/>
+    </row>
+    <row r="10" spans="1:27" ht="29.25" hidden="1" customHeight="1">
+      <c r="A10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="32" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -3364,46 +3344,46 @@
       <c r="E10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="33">
         <v>13</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="33">
         <v>1</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M10" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="L10" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M10" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="41"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="41"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-    </row>
-    <row r="11" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+    </row>
+    <row r="11" spans="1:27" ht="27.6" hidden="1">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -3419,46 +3399,46 @@
       <c r="E11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="25">
         <v>13</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="25">
         <v>1</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M11" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="L11" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M11" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="41"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
-    </row>
-    <row r="12" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="39"/>
+      <c r="Y11" s="39"/>
+      <c r="Z11" s="39"/>
+      <c r="AA11" s="39"/>
+    </row>
+    <row r="12" spans="1:27" ht="27.6" hidden="1">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -3489,31 +3469,31 @@
       <c r="J12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="37" t="s">
+      <c r="K12" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M12" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="L12" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="60"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-    </row>
-    <row r="13" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39"/>
+      <c r="Z12" s="39"/>
+      <c r="AA12" s="39"/>
+    </row>
+    <row r="13" spans="1:27" ht="27.6" hidden="1">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -3544,31 +3524,31 @@
       <c r="J13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="37" t="s">
-        <v>191</v>
+      <c r="K13" s="35" t="s">
+        <v>190</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-    </row>
-    <row r="14" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+    </row>
+    <row r="14" spans="1:27" ht="27.6" hidden="1">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -3599,31 +3579,31 @@
       <c r="J14" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="37" t="s">
-        <v>192</v>
+      <c r="K14" s="35" t="s">
+        <v>191</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="60"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
-    </row>
-    <row r="15" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+    </row>
+    <row r="15" spans="1:27" ht="27.6" hidden="1">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -3654,31 +3634,31 @@
       <c r="J15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="37" t="s">
-        <v>193</v>
+      <c r="K15" s="35" t="s">
+        <v>192</v>
       </c>
       <c r="L15" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M15" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M15" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-    </row>
-    <row r="16" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="39"/>
+      <c r="X15" s="39"/>
+      <c r="Y15" s="39"/>
+      <c r="Z15" s="39"/>
+      <c r="AA15" s="39"/>
+    </row>
+    <row r="16" spans="1:27" ht="27.6" hidden="1">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -3709,31 +3689,31 @@
       <c r="J16" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="37" t="s">
-        <v>194</v>
+      <c r="K16" s="35" t="s">
+        <v>193</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="41"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="41"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="41"/>
-      <c r="Y16" s="41"/>
-      <c r="Z16" s="41"/>
-      <c r="AA16" s="41"/>
-    </row>
-    <row r="17" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+    </row>
+    <row r="17" spans="1:27" ht="29.25" hidden="1" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
@@ -3764,35 +3744,35 @@
       <c r="J17" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="37" t="s">
-        <v>195</v>
+      <c r="K17" s="35" t="s">
+        <v>194</v>
       </c>
       <c r="L17" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M17" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="63" t="s">
+      <c r="Q17" s="51"/>
+      <c r="R17" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="S17" s="64"/>
-      <c r="T17" s="41"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="41"/>
-    </row>
-    <row r="18" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S17" s="62"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="39"/>
+      <c r="Z17" s="39"/>
+      <c r="AA17" s="39"/>
+    </row>
+    <row r="18" spans="1:27" ht="27.6">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -3811,7 +3791,7 @@
       <c r="F18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="36">
+      <c r="G18" s="34">
         <v>5</v>
       </c>
       <c r="H18" s="2">
@@ -3820,43 +3800,43 @@
       <c r="I18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K18" s="37" t="s">
-        <v>196</v>
+      <c r="K18" s="35" t="s">
+        <v>195</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="Q18" s="42">
+      <c r="Q18" s="40">
         <f>SUM(Q19:Q21)</f>
         <v>532</v>
       </c>
-      <c r="R18" s="43" t="s">
+      <c r="R18" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="S18" s="43">
+      <c r="S18" s="41">
         <v>370</v>
       </c>
-      <c r="T18" s="41"/>
-      <c r="U18" s="41"/>
-      <c r="V18" s="41"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="41"/>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="41"/>
-    </row>
-    <row r="19" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
+      <c r="W18" s="39"/>
+      <c r="X18" s="39"/>
+      <c r="Y18" s="39"/>
+      <c r="Z18" s="39"/>
+      <c r="AA18" s="39"/>
+    </row>
+    <row r="19" spans="1:27" ht="27.6">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -3884,51 +3864,51 @@
       <c r="I19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="37" t="s">
-        <v>197</v>
+      <c r="K19" s="35" t="s">
+        <v>196</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M19" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q19" s="44">
+        <v>177</v>
+      </c>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q19" s="42">
         <f>SUM(G34:G69)</f>
         <v>196</v>
       </c>
-      <c r="R19" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="S19" s="45">
+      <c r="R19" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="S19" s="43">
         <v>150</v>
       </c>
-      <c r="T19" s="41"/>
-      <c r="U19" s="41"/>
-      <c r="V19" s="41"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="41"/>
-      <c r="Z19" s="41"/>
-      <c r="AA19" s="41"/>
-    </row>
-    <row r="20" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T19" s="39"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="39"/>
+      <c r="Y19" s="39"/>
+      <c r="Z19" s="39"/>
+      <c r="AA19" s="39"/>
+    </row>
+    <row r="20" spans="1:27" ht="27.6">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>14</v>
@@ -3948,43 +3928,43 @@
       <c r="I20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="37" t="s">
-        <v>198</v>
+      <c r="J20" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>197</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M20" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="Q20" s="47">
+      <c r="Q20" s="45">
         <f>SUM(G18:G33)</f>
         <v>178</v>
       </c>
-      <c r="R20" s="45" t="s">
+      <c r="R20" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="S20" s="45">
+      <c r="S20" s="43">
         <v>100</v>
       </c>
-      <c r="T20" s="41"/>
-      <c r="U20" s="41"/>
-      <c r="V20" s="41"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="41"/>
-      <c r="Y20" s="41"/>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="41"/>
-    </row>
-    <row r="21" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+    </row>
+    <row r="21" spans="1:27" ht="27.6">
       <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
@@ -3992,7 +3972,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>14</v>
@@ -4012,43 +3992,43 @@
       <c r="I21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="37" t="s">
-        <v>199</v>
+      <c r="K21" s="35" t="s">
+        <v>198</v>
       </c>
       <c r="L21" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M21" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M21" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="48" t="s">
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" s="49">
+      <c r="Q21" s="47">
         <f>SUM(G3:G17)</f>
         <v>158</v>
       </c>
-      <c r="R21" s="45" t="s">
+      <c r="R21" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="S21" s="45">
+      <c r="S21" s="43">
         <v>50</v>
       </c>
-      <c r="T21" s="41"/>
-      <c r="U21" s="41"/>
-      <c r="V21" s="41"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="41"/>
-      <c r="Y21" s="41"/>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="41"/>
-    </row>
-    <row r="22" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="39"/>
+      <c r="Z21" s="39"/>
+      <c r="AA21" s="39"/>
+    </row>
+    <row r="22" spans="1:27" ht="27.6">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -4056,7 +4036,7 @@
         <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>14</v>
@@ -4076,39 +4056,39 @@
       <c r="I22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J22" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="37" t="s">
-        <v>200</v>
+      <c r="J22" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K22" s="35" t="s">
+        <v>199</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="50" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q22" s="51">
+        <v>185</v>
+      </c>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q22" s="49">
         <f>AVERAGE(Q19:Q21)</f>
         <v>177.33333333333334</v>
       </c>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="41"/>
-      <c r="U22" s="41"/>
-      <c r="V22" s="41"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="41"/>
-      <c r="Z22" s="41"/>
-      <c r="AA22" s="41"/>
-    </row>
-    <row r="23" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="39"/>
+      <c r="U22" s="39"/>
+      <c r="V22" s="39"/>
+      <c r="W22" s="39"/>
+      <c r="X22" s="39"/>
+      <c r="Y22" s="39"/>
+      <c r="Z22" s="39"/>
+      <c r="AA22" s="39"/>
+    </row>
+    <row r="23" spans="1:27" ht="27.6">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -4116,7 +4096,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>14</v>
@@ -4136,42 +4116,42 @@
       <c r="I23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K23" s="37" t="s">
-        <v>201</v>
+      <c r="J23" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="35" t="s">
+        <v>200</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M23" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="41"/>
-      <c r="U23" s="41"/>
-      <c r="V23" s="41"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="41"/>
-      <c r="Z23" s="41"/>
-      <c r="AA23" s="41"/>
-    </row>
-    <row r="24" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="39"/>
+      <c r="X23" s="39"/>
+      <c r="Y23" s="39"/>
+      <c r="Z23" s="39"/>
+      <c r="AA23" s="39"/>
+    </row>
+    <row r="24" spans="1:27" ht="27.6">
       <c r="A24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>24</v>
@@ -4191,48 +4171,48 @@
       <c r="I24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K24" s="37" t="s">
-        <v>202</v>
+      <c r="J24" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>201</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
-      <c r="T24" s="41"/>
-      <c r="U24" s="41"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="41"/>
-      <c r="Y24" s="41"/>
-      <c r="Z24" s="41"/>
-      <c r="AA24" s="41"/>
-    </row>
-    <row r="25" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="39"/>
+      <c r="U24" s="39"/>
+      <c r="V24" s="39"/>
+      <c r="W24" s="39"/>
+      <c r="X24" s="39"/>
+      <c r="Y24" s="39"/>
+      <c r="Z24" s="39"/>
+      <c r="AA24" s="39"/>
+    </row>
+    <row r="25" spans="1:27" ht="27.6">
       <c r="A25" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>16</v>
@@ -4246,48 +4226,48 @@
       <c r="I25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="J25" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K25" s="37" t="s">
-        <v>203</v>
+      <c r="K25" s="35" t="s">
+        <v>202</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="41"/>
-      <c r="U25" s="41"/>
-      <c r="V25" s="41"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="41"/>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="41"/>
-    </row>
-    <row r="26" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="39"/>
+      <c r="V25" s="39"/>
+      <c r="W25" s="39"/>
+      <c r="X25" s="39"/>
+      <c r="Y25" s="39"/>
+      <c r="Z25" s="39"/>
+      <c r="AA25" s="39"/>
+    </row>
+    <row r="26" spans="1:27" ht="27.6">
       <c r="A26" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>21</v>
@@ -4301,34 +4281,34 @@
       <c r="I26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" s="37" t="s">
-        <v>204</v>
+      <c r="J26" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K26" s="35" t="s">
+        <v>203</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
-      <c r="T26" s="41"/>
-      <c r="U26" s="41"/>
-      <c r="V26" s="41"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="41"/>
-      <c r="Y26" s="41"/>
-      <c r="Z26" s="41"/>
-      <c r="AA26" s="41"/>
-    </row>
-    <row r="27" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="39"/>
+      <c r="T26" s="39"/>
+      <c r="U26" s="39"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="39"/>
+      <c r="Y26" s="39"/>
+      <c r="Z26" s="39"/>
+      <c r="AA26" s="39"/>
+    </row>
+    <row r="27" spans="1:27" ht="29.25" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -4336,10 +4316,10 @@
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>15</v>
@@ -4356,34 +4336,34 @@
       <c r="I27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J27" s="23" t="s">
+      <c r="J27" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="37" t="s">
-        <v>205</v>
+      <c r="K27" s="35" t="s">
+        <v>204</v>
       </c>
       <c r="L27" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M27" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M27" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="41"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="41"/>
-      <c r="U27" s="41"/>
-      <c r="V27" s="41"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="41"/>
-      <c r="Y27" s="41"/>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="41"/>
-    </row>
-    <row r="28" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
+      <c r="T27" s="39"/>
+      <c r="U27" s="39"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="39"/>
+      <c r="Y27" s="39"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="39"/>
+    </row>
+    <row r="28" spans="1:27" ht="27.6">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -4391,7 +4371,7 @@
         <v>37</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>14</v>
@@ -4411,34 +4391,34 @@
       <c r="I28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K28" s="37" t="s">
-        <v>206</v>
+      <c r="J28" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>205</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="41"/>
-      <c r="V28" s="41"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="41"/>
-    </row>
-    <row r="29" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="39"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="39"/>
+      <c r="Y28" s="39"/>
+      <c r="Z28" s="39"/>
+      <c r="AA28" s="39"/>
+    </row>
+    <row r="29" spans="1:27" ht="27.6">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -4446,7 +4426,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>14</v>
@@ -4466,42 +4446,42 @@
       <c r="I29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="J29" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K29" s="37" t="s">
-        <v>207</v>
+      <c r="K29" s="35" t="s">
+        <v>206</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="41"/>
-      <c r="V29" s="41"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="41"/>
-      <c r="Z29" s="41"/>
-      <c r="AA29" s="41"/>
-    </row>
-    <row r="30" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
+      <c r="R29" s="39"/>
+      <c r="S29" s="39"/>
+      <c r="T29" s="39"/>
+      <c r="U29" s="39"/>
+      <c r="V29" s="39"/>
+      <c r="W29" s="39"/>
+      <c r="X29" s="39"/>
+      <c r="Y29" s="39"/>
+      <c r="Z29" s="39"/>
+      <c r="AA29" s="39"/>
+    </row>
+    <row r="30" spans="1:27" ht="27.6">
       <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>14</v>
@@ -4521,42 +4501,42 @@
       <c r="I30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K30" s="37" t="s">
-        <v>208</v>
+      <c r="K30" s="35" t="s">
+        <v>207</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="41"/>
-      <c r="V30" s="41"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="41"/>
-      <c r="Y30" s="41"/>
-      <c r="Z30" s="41"/>
-      <c r="AA30" s="41"/>
-    </row>
-    <row r="31" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="39"/>
+      <c r="R30" s="39"/>
+      <c r="S30" s="39"/>
+      <c r="T30" s="39"/>
+      <c r="U30" s="39"/>
+      <c r="V30" s="39"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="39"/>
+      <c r="Z30" s="39"/>
+      <c r="AA30" s="39"/>
+    </row>
+    <row r="31" spans="1:27" ht="27.6">
       <c r="A31" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>14</v>
@@ -4576,47 +4556,47 @@
       <c r="I31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J31" s="23" t="s">
+      <c r="J31" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K31" s="37" t="s">
-        <v>209</v>
+      <c r="K31" s="35" t="s">
+        <v>208</v>
       </c>
       <c r="L31" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M31" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="41"/>
-      <c r="V31" s="41"/>
-      <c r="W31" s="41"/>
-      <c r="X31" s="41"/>
-      <c r="Y31" s="41"/>
-      <c r="Z31" s="41"/>
-      <c r="AA31" s="41"/>
-    </row>
-    <row r="32" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="39"/>
+      <c r="R31" s="39"/>
+      <c r="S31" s="39"/>
+      <c r="T31" s="39"/>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="39"/>
+      <c r="Z31" s="39"/>
+      <c r="AA31" s="39"/>
+    </row>
+    <row r="32" spans="1:27" ht="27.6">
       <c r="A32" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="2" t="s">
@@ -4631,42 +4611,42 @@
       <c r="I32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="66" t="s">
+      <c r="J32" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K32" s="37" t="s">
-        <v>210</v>
+      <c r="K32" s="35" t="s">
+        <v>209</v>
       </c>
       <c r="L32" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="N32" s="41"/>
-      <c r="O32" s="41"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="41"/>
-      <c r="T32" s="41"/>
-      <c r="U32" s="41"/>
-      <c r="V32" s="41"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="41"/>
-      <c r="Y32" s="41"/>
-      <c r="Z32" s="41"/>
-      <c r="AA32" s="41"/>
-    </row>
-    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="39"/>
+    </row>
+    <row r="33" spans="1:13" ht="27.6">
       <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>14</v>
@@ -4686,28 +4666,28 @@
       <c r="I33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J33" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33" s="37" t="s">
-        <v>211</v>
+      <c r="J33" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K33" s="35" t="s">
+        <v>210</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M33" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="27.6" hidden="1">
       <c r="A34" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>14</v>
@@ -4725,30 +4705,30 @@
         <v>3</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J34" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K34" s="37" t="s">
-        <v>212</v>
+      <c r="K34" s="35" t="s">
+        <v>211</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="41.4" hidden="1">
       <c r="A35" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>14</v>
@@ -4766,30 +4746,30 @@
         <v>3</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J35" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K35" s="37" t="s">
-        <v>213</v>
+      <c r="K35" s="35" t="s">
+        <v>212</v>
       </c>
       <c r="L35" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="27.6" hidden="1">
       <c r="A36" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="C36" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>14</v>
@@ -4807,30 +4787,30 @@
         <v>3</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J36" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K36" s="37" t="s">
-        <v>214</v>
+      <c r="K36" s="35" t="s">
+        <v>213</v>
       </c>
       <c r="L36" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M36" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M36" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:13" ht="27.6" hidden="1">
       <c r="A37" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>14</v>
@@ -4848,30 +4828,30 @@
         <v>3</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J37" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K37" s="37" t="s">
-        <v>215</v>
+      <c r="K37" s="35" t="s">
+        <v>214</v>
       </c>
       <c r="L37" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>14</v>
@@ -4889,30 +4869,30 @@
         <v>2</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J38" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K38" s="37" t="s">
-        <v>216</v>
+      <c r="K38" s="35" t="s">
+        <v>215</v>
       </c>
       <c r="L38" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M38" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>14</v>
@@ -4930,30 +4910,30 @@
         <v>2</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J39" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K39" s="37" t="s">
-        <v>217</v>
+      <c r="K39" s="35" t="s">
+        <v>216</v>
       </c>
       <c r="L39" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M39" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>106</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>14</v>
@@ -4971,30 +4951,30 @@
         <v>1</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J40" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K40" s="37" t="s">
-        <v>218</v>
+      <c r="K40" s="35" t="s">
+        <v>217</v>
       </c>
       <c r="L40" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M40" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>24</v>
@@ -5012,30 +4992,30 @@
         <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J41" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K41" s="37" t="s">
-        <v>219</v>
+      <c r="K41" s="35" t="s">
+        <v>218</v>
       </c>
       <c r="L41" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M41" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>24</v>
@@ -5053,33 +5033,33 @@
         <v>1</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J42" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K42" s="37" t="s">
-        <v>220</v>
+      <c r="K42" s="35" t="s">
+        <v>219</v>
       </c>
       <c r="L42" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M42" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="27.6" hidden="1">
       <c r="A43" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="D43" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E43" s="20" t="s">
         <v>15</v>
@@ -5094,30 +5074,30 @@
         <v>1</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J43" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K43" s="37" t="s">
-        <v>221</v>
+      <c r="K43" s="35" t="s">
+        <v>220</v>
       </c>
       <c r="L43" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M43" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="27.6" hidden="1">
       <c r="A44" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="C44" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>14</v>
@@ -5135,30 +5115,30 @@
         <v>3</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J44" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K44" s="37" t="s">
-        <v>222</v>
+      <c r="K44" s="35" t="s">
+        <v>221</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M44" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="27.6" hidden="1">
       <c r="A45" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>24</v>
@@ -5176,30 +5156,30 @@
         <v>3</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J45" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K45" s="37" t="s">
-        <v>223</v>
+      <c r="K45" s="35" t="s">
+        <v>222</v>
       </c>
       <c r="L45" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M45" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="27.6" hidden="1">
       <c r="A46" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>24</v>
@@ -5217,30 +5197,30 @@
         <v>3</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J46" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K46" s="37" t="s">
-        <v>224</v>
+      <c r="K46" s="35" t="s">
+        <v>223</v>
       </c>
       <c r="L46" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M46" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M46" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:13" ht="27.6" hidden="1">
       <c r="A47" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="C47" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>24</v>
@@ -5258,30 +5238,30 @@
         <v>3</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J47" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K47" s="37" t="s">
-        <v>225</v>
+      <c r="K47" s="35" t="s">
+        <v>224</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M47" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="27.6" hidden="1">
       <c r="A48" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>14</v>
@@ -5299,30 +5279,30 @@
         <v>3</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J48" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K48" s="37" t="s">
-        <v>226</v>
+      <c r="K48" s="35" t="s">
+        <v>225</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M48" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="27.6" hidden="1">
       <c r="A49" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B49" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>126</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>14</v>
@@ -5340,30 +5320,30 @@
         <v>2</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J49" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K49" s="37" t="s">
-        <v>227</v>
+      <c r="K49" s="35" t="s">
+        <v>226</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M49" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A50" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>14</v>
@@ -5381,30 +5361,30 @@
         <v>1</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J50" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K50" s="37" t="s">
-        <v>228</v>
+      <c r="K50" s="35" t="s">
+        <v>227</v>
       </c>
       <c r="L50" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M50" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="27.6" hidden="1">
       <c r="A51" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>14</v>
@@ -5422,30 +5402,30 @@
         <v>2</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J51" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K51" s="37" t="s">
-        <v>229</v>
+      <c r="K51" s="35" t="s">
+        <v>228</v>
       </c>
       <c r="L51" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M51" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A52" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>14</v>
@@ -5463,30 +5443,30 @@
         <v>2</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J52" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K52" s="37" t="s">
-        <v>230</v>
+      <c r="K52" s="35" t="s">
+        <v>229</v>
       </c>
       <c r="L52" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M52" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A53" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>14</v>
@@ -5504,30 +5484,30 @@
         <v>2</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J53" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K53" s="37" t="s">
-        <v>231</v>
+      <c r="K53" s="35" t="s">
+        <v>230</v>
       </c>
       <c r="L53" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M53" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A54" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>14</v>
@@ -5545,30 +5525,30 @@
         <v>3</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J54" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K54" s="37" t="s">
-        <v>232</v>
+      <c r="K54" s="35" t="s">
+        <v>231</v>
       </c>
       <c r="L54" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M54" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M54" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A55" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>24</v>
@@ -5586,36 +5566,36 @@
         <v>1</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J55" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K55" s="37" t="s">
-        <v>233</v>
+      <c r="K55" s="35" t="s">
+        <v>232</v>
       </c>
       <c r="L55" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M55" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A56" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>16</v>
@@ -5627,36 +5607,36 @@
         <v>2</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J56" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K56" s="37" t="s">
-        <v>234</v>
+      <c r="K56" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="L56" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M56" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A57" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>21</v>
@@ -5668,36 +5648,36 @@
         <v>2</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J57" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K57" s="37" t="s">
-        <v>235</v>
+      <c r="K57" s="35" t="s">
+        <v>234</v>
       </c>
       <c r="L57" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M57" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A58" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>24</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>16</v>
@@ -5709,30 +5689,30 @@
         <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J58" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K58" s="37" t="s">
-        <v>236</v>
+      <c r="K58" s="35" t="s">
+        <v>235</v>
       </c>
       <c r="L58" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M58" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="27.6" hidden="1">
       <c r="A59" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B59" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>14</v>
@@ -5750,30 +5730,30 @@
         <v>3</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J59" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K59" s="37" t="s">
-        <v>237</v>
+      <c r="K59" s="35" t="s">
+        <v>236</v>
       </c>
       <c r="L59" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M59" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M59" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:13" ht="27.6" hidden="1">
       <c r="A60" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>146</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>14</v>
@@ -5791,30 +5771,30 @@
         <v>3</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J60" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K60" s="37" t="s">
-        <v>238</v>
+      <c r="K60" s="35" t="s">
+        <v>237</v>
       </c>
       <c r="L60" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M60" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="27.6" hidden="1">
       <c r="A61" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>24</v>
@@ -5832,30 +5812,30 @@
         <v>2</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J61" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K61" s="37" t="s">
-        <v>239</v>
+      <c r="K61" s="35" t="s">
+        <v>238</v>
       </c>
       <c r="L61" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M61" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A62" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B62" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D62" s="11" t="s">
         <v>24</v>
@@ -5873,30 +5853,30 @@
         <v>2</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J62" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K62" s="37" t="s">
-        <v>230</v>
+      <c r="K62" s="35" t="s">
+        <v>229</v>
       </c>
       <c r="L62" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M62" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A63" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>24</v>
@@ -5914,30 +5894,30 @@
         <v>1</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J63" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K63" s="37" t="s">
-        <v>231</v>
+      <c r="K63" s="35" t="s">
+        <v>230</v>
       </c>
       <c r="L63" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M63" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="29.25" hidden="1" customHeight="1">
       <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B64" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>24</v>
@@ -5955,30 +5935,30 @@
         <v>2</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J64" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K64" s="37" t="s">
-        <v>232</v>
+      <c r="K64" s="35" t="s">
+        <v>231</v>
       </c>
       <c r="L64" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M64" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="27.6" hidden="1">
       <c r="A65" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="C65" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>14</v>
@@ -5996,30 +5976,30 @@
         <v>3</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J65" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K65" s="37" t="s">
-        <v>233</v>
+      <c r="K65" s="35" t="s">
+        <v>232</v>
       </c>
       <c r="L65" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M65" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="41.4" hidden="1">
       <c r="A66" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="C66" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>14</v>
@@ -6037,30 +6017,30 @@
         <v>3</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J66" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K66" s="37" t="s">
-        <v>234</v>
+      <c r="K66" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M66" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="27.6" hidden="1">
       <c r="A67" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>14</v>
@@ -6078,30 +6058,30 @@
         <v>3</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J67" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K67" s="37" t="s">
-        <v>235</v>
+      <c r="K67" s="35" t="s">
+        <v>234</v>
       </c>
       <c r="L67" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M67" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="27.6" hidden="1">
       <c r="A68" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="D68" s="11" t="s">
         <v>14</v>
@@ -6119,30 +6099,30 @@
         <v>2</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J68" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K68" s="37" t="s">
-        <v>236</v>
+      <c r="K68" s="35" t="s">
+        <v>235</v>
       </c>
       <c r="L68" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M68" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="M68" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:13" ht="27.6" hidden="1">
       <c r="A69" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B69" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>14</v>
@@ -6160,26 +6140,33 @@
         <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J69" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K69" s="37" t="s">
-        <v>237</v>
+      <c r="K69" s="35" t="s">
+        <v>236</v>
       </c>
       <c r="L69" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M69" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="I70" s="18"/>
       <c r="J70" s="18"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AA69" xr:uid="{7D7E9CD4-C5BF-4C2C-BA24-C51E067CFB1E}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="SP2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="9">
     <mergeCell ref="N14:S14"/>
     <mergeCell ref="A1:J1"/>
@@ -6192,6 +6179,7 @@
     <mergeCell ref="N13:S13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>